<commit_message>
Update publications and encoding check notebooks; adjust Python environment and version
</commit_message>
<xml_diff>
--- a/markdown_generator/publications_dictionary.xlsx
+++ b/markdown_generator/publications_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcd_ncckl9u\Documents\GitHub\marcdordal.github.io\markdown_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Documents\GitHub\marcdordal.github.io\markdown_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BB6B0D-C33C-431F-8DFA-20E1D7AC089D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9580724C-5A6A-4913-97D7-F6AC150A8E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{04DE6DD2-1E98-49E4-98A9-412003E60FA6}"/>
+    <workbookView xWindow="3450" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{04DE6DD2-1E98-49E4-98A9-412003E60FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Variable</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>string, text to display on download hyperlink of optional file</t>
+  </si>
+  <si>
+    <t>reject_resubmit</t>
   </si>
 </sst>
 </file>
@@ -329,9 +332,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -369,7 +372,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -475,7 +478,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -617,7 +620,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -625,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E468A78A-65AD-47CF-BE48-BF2498C04D25}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,111 +710,117 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 'Reject and Resubmit' status handling and update execution counts in publications
</commit_message>
<xml_diff>
--- a/markdown_generator/publications_dictionary.xlsx
+++ b/markdown_generator/publications_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Documents\GitHub\marcdordal.github.io\markdown_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9580724C-5A6A-4913-97D7-F6AC150A8E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B4051D-94A2-4150-88CC-9B5C9D8122AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3450" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{04DE6DD2-1E98-49E4-98A9-412003E60FA6}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>